<commit_message>
Updated D3 to 100V rating (BOM change on Jan 26, 2017)
</commit_message>
<xml_diff>
--- a/DSIB-BOM.xlsx
+++ b/DSIB-BOM.xlsx
@@ -22,10 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="261">
-  <si>
-    <t>dSIB  Revised: Tuesday, October 04, 2016</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="261">
   <si>
     <t>Intuitive Surgical, Inc.</t>
   </si>
@@ -270,15 +267,6 @@
     <t>D3</t>
   </si>
   <si>
-    <t>ZHCS750/SOT</t>
-  </si>
-  <si>
-    <t>ZHCS750TA</t>
-  </si>
-  <si>
-    <t>ZHCS750CT-ND</t>
-  </si>
-  <si>
     <t>SM/SOT23_123</t>
   </si>
   <si>
@@ -804,7 +792,19 @@
     <t>330uH 130mA</t>
   </si>
   <si>
-    <t>Bill Of Materials        October 4, 2016      13:28:36</t>
+    <t>BAR46FILM</t>
+  </si>
+  <si>
+    <t>ST Micro</t>
+  </si>
+  <si>
+    <t>497-12128-1-ND</t>
+  </si>
+  <si>
+    <t>dSIB  Revised: January 26, 2017</t>
+  </si>
+  <si>
+    <t>Bill Of Materials       January 26, 2017</t>
   </si>
 </sst>
 </file>
@@ -1669,7 +1669,7 @@
   <dimension ref="A1:K63"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="70" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1690,14 +1690,14 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>0</v>
+        <v>259</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -1709,21 +1709,21 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -1742,37 +1742,37 @@
     </row>
     <row r="10" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="C10" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="F10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="G10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="H10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="I10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="I10" s="2" t="s">
+      <c r="J10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="J10" s="2" t="s">
+      <c r="K10" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="K10" s="2" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -1783,31 +1783,31 @@
         <v>7</v>
       </c>
       <c r="C11" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="E11" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="F11" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F11" s="3" t="s">
-        <v>17</v>
-      </c>
       <c r="G11" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H11" s="3" t="s">
+      <c r="I11" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I11" s="3" t="s">
+      <c r="J11" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J11" s="3" t="s">
+      <c r="K11" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="K11" s="3" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -1818,31 +1818,31 @@
         <v>2</v>
       </c>
       <c r="C12" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>24</v>
-      </c>
       <c r="E12" s="3" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="I12" s="3">
         <v>177303</v>
       </c>
       <c r="J12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K12" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="K12" s="3" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -1853,31 +1853,31 @@
         <v>6</v>
       </c>
       <c r="C13" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="E13" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F13" s="3" t="s">
+      <c r="G13" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H13" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G13" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H13" s="3" t="s">
+      <c r="I13" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J13" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="I13" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="J13" s="3" t="s">
-        <v>32</v>
-      </c>
       <c r="K13" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -1888,31 +1888,31 @@
         <v>2</v>
       </c>
       <c r="C14" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="E14" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="F14" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="G14" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H14" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="G14" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H14" s="3" t="s">
+      <c r="I14" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K14" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="I14" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="J14" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="K14" s="3" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
@@ -1923,31 +1923,31 @@
         <v>3</v>
       </c>
       <c r="C15" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="E15" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="E15" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F15" s="3" t="s">
+      <c r="G15" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H15" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="G15" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>42</v>
-      </c>
       <c r="I15" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
@@ -1958,31 +1958,31 @@
         <v>80</v>
       </c>
       <c r="C16" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F16" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F16" s="3" t="s">
+      <c r="G16" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H16" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="G16" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H16" s="3" t="s">
+      <c r="I16" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J16" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="I16" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="J16" s="3" t="s">
+      <c r="K16" s="3" t="s">
         <v>46</v>
-      </c>
-      <c r="K16" s="3" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
@@ -1993,31 +1993,31 @@
         <v>1</v>
       </c>
       <c r="C17" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E17" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D17" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E17" s="3" t="s">
+      <c r="F17" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="G17" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H17" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="G17" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H17" s="3" t="s">
+      <c r="I17" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J17" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="I17" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="J17" s="3" t="s">
-        <v>52</v>
-      </c>
       <c r="K17" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
@@ -2028,31 +2028,31 @@
         <v>2</v>
       </c>
       <c r="C18" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D18" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="E18" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F18" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="E18" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="F18" s="3" t="s">
+      <c r="G18" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H18" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="G18" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>56</v>
-      </c>
       <c r="I18" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
@@ -2063,31 +2063,31 @@
         <v>2</v>
       </c>
       <c r="C19" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D19" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="E19" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F19" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="E19" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F19" s="3" t="s">
+      <c r="G19" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H19" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="G19" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>60</v>
-      </c>
       <c r="I19" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J19" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J19" s="3" t="s">
-        <v>21</v>
-      </c>
       <c r="K19" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
@@ -2098,31 +2098,31 @@
         <v>60</v>
       </c>
       <c r="C20" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D20" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="E20" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F20" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="E20" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F20" s="3" t="s">
+      <c r="G20" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H20" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="G20" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>64</v>
-      </c>
       <c r="I20" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K20" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
@@ -2133,31 +2133,31 @@
         <v>2</v>
       </c>
       <c r="C21" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D21" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="E21" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J21" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E21" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H21" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="I21" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="J21" s="3" t="s">
-        <v>67</v>
-      </c>
       <c r="K21" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
@@ -2168,31 +2168,31 @@
         <v>4</v>
       </c>
       <c r="C22" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D22" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="E22" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F22" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="E22" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F22" s="3" t="s">
+      <c r="G22" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H22" s="3" t="s">
         <v>70</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H22" s="3" t="s">
-        <v>71</v>
       </c>
       <c r="I22" s="3">
         <v>177623</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
@@ -2203,31 +2203,31 @@
         <v>1</v>
       </c>
       <c r="C23" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F23" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="D23" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F23" s="3" t="s">
+      <c r="G23" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H23" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="G23" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H23" s="3" t="s">
+      <c r="I23" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K23" s="3" t="s">
         <v>74</v>
-      </c>
-      <c r="I23" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="J23" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="K23" s="3" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
@@ -2238,28 +2238,28 @@
         <v>2</v>
       </c>
       <c r="C24" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D24" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="E24" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="E24" s="3" t="s">
+      <c r="F24" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H24" s="3" t="s">
         <v>78</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="G24" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H24" s="3" t="s">
-        <v>79</v>
       </c>
       <c r="I24" s="3">
         <v>173257</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K24" s="3"/>
     </row>
@@ -2271,30 +2271,32 @@
         <v>1</v>
       </c>
       <c r="C25" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J25" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="D25" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H25" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="I25" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="J25" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="K25" s="3"/>
+      <c r="K25" s="3" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
@@ -2304,28 +2306,28 @@
         <v>4</v>
       </c>
       <c r="C26" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H26" s="3" t="s">
         <v>92</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="G26" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H26" s="3" t="s">
-        <v>96</v>
       </c>
       <c r="I26" s="3">
         <v>180373</v>
       </c>
       <c r="J26" s="3" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="K26" s="3"/>
     </row>
@@ -2337,28 +2339,28 @@
         <v>1</v>
       </c>
       <c r="C27" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="G27" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="H27" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="E27" s="3" t="s">
+      <c r="I27" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J27" s="3" t="s">
         <v>99</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="G27" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="H27" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="I27" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="J27" s="3" t="s">
-        <v>103</v>
       </c>
       <c r="K27" s="3"/>
     </row>
@@ -2370,26 +2372,26 @@
         <v>1</v>
       </c>
       <c r="C28" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H28" s="3" t="s">
         <v>104</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H28" s="3" t="s">
-        <v>108</v>
       </c>
       <c r="I28" s="3"/>
       <c r="J28" s="3" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="K28" s="3"/>
     </row>
@@ -2401,26 +2403,26 @@
         <v>4</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="F29" s="3">
         <v>61300311121</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="I29" s="3"/>
       <c r="J29" s="3" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="K29" s="3"/>
     </row>
@@ -2432,26 +2434,26 @@
         <v>1</v>
       </c>
       <c r="C30" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H30" s="3" t="s">
         <v>115</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="G30" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H30" s="3" t="s">
-        <v>119</v>
       </c>
       <c r="I30" s="3"/>
       <c r="J30" s="3" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="K30" s="3"/>
     </row>
@@ -2463,28 +2465,28 @@
         <v>4</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="F31" s="3">
         <v>74437336022</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J31" s="3" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="K31" s="3"/>
     </row>
@@ -2496,28 +2498,28 @@
         <v>3</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J32" s="3" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="K32" s="3"/>
     </row>
@@ -2529,28 +2531,28 @@
         <v>2</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="D33" s="3">
         <v>100</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="I33" s="3">
         <v>178019</v>
       </c>
       <c r="J33" s="3" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="K33" s="3"/>
     </row>
@@ -2562,28 +2564,28 @@
         <v>2</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D34" s="3">
         <v>1.2E-2</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="I34" s="3">
         <v>178033</v>
       </c>
       <c r="J34" s="3" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="K34" s="3"/>
     </row>
@@ -2595,28 +2597,28 @@
         <v>1</v>
       </c>
       <c r="C35" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H35" s="3" t="s">
         <v>136</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="F35" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="G35" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H35" s="3" t="s">
-        <v>140</v>
       </c>
       <c r="I35" s="3">
         <v>179408</v>
       </c>
       <c r="J35" s="3" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="K35" s="3"/>
     </row>
@@ -2628,28 +2630,28 @@
         <v>1</v>
       </c>
       <c r="C36" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H36" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="D36" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="E36" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="F36" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="G36" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H36" s="3" t="s">
-        <v>146</v>
-      </c>
       <c r="I36" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J36" s="3" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="K36" s="3"/>
     </row>
@@ -2661,28 +2663,28 @@
         <v>81</v>
       </c>
       <c r="C37" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H37" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="D37" s="3" t="s">
+      <c r="I37" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J37" s="3" t="s">
         <v>148</v>
-      </c>
-      <c r="E37" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="F37" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="G37" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H37" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="I37" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="J37" s="3" t="s">
-        <v>152</v>
       </c>
       <c r="K37" s="3"/>
     </row>
@@ -2694,28 +2696,28 @@
         <v>9</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="I38" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J38" s="3" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="K38" s="3"/>
     </row>
@@ -2727,28 +2729,28 @@
         <v>1</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="I39" s="3">
         <v>179617</v>
       </c>
       <c r="J39" s="3" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="K39" s="3"/>
     </row>
@@ -2760,28 +2762,28 @@
         <v>10</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="I40" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J40" s="3" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="K40" s="3"/>
     </row>
@@ -2793,28 +2795,28 @@
         <v>2</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="D41" s="3">
         <v>49.9</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="I41" s="3">
         <v>179621</v>
       </c>
       <c r="J41" s="3" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="K41" s="3"/>
     </row>
@@ -2826,28 +2828,28 @@
         <v>1</v>
       </c>
       <c r="C42" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="G42" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H42" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="I42" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J42" s="3" t="s">
         <v>166</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="E42" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="F42" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="G42" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H42" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="I42" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="J42" s="3" t="s">
-        <v>170</v>
       </c>
       <c r="K42" s="3"/>
     </row>
@@ -2859,28 +2861,28 @@
         <v>4</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H43" s="3" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="I43" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J43" s="3" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="K43" s="3"/>
     </row>
@@ -2892,28 +2894,28 @@
         <v>4</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H44" s="3" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="I44" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J44" s="3" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="K44" s="3"/>
     </row>
@@ -2925,28 +2927,28 @@
         <v>1</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H45" s="3" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="I45" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J45" s="3" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="K45" s="3"/>
     </row>
@@ -2958,26 +2960,26 @@
         <v>12</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H46" s="3" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="I46" s="3"/>
       <c r="J46" s="3" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="K46" s="3"/>
     </row>
@@ -2989,28 +2991,28 @@
         <v>1</v>
       </c>
       <c r="C47" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="G47" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H47" s="3" t="s">
         <v>197</v>
-      </c>
-      <c r="D47" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="E47" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="F47" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="G47" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H47" s="3" t="s">
-        <v>201</v>
       </c>
       <c r="I47" s="3">
         <v>171923</v>
       </c>
       <c r="J47" s="3" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="K47" s="3"/>
     </row>
@@ -3022,28 +3024,28 @@
         <v>1</v>
       </c>
       <c r="C48" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="F48" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="G48" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H48" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="D48" s="3" t="s">
+      <c r="I48" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J48" s="3" t="s">
         <v>204</v>
-      </c>
-      <c r="E48" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="F48" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="G48" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H48" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="I48" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="J48" s="3" t="s">
-        <v>208</v>
       </c>
       <c r="K48" s="3"/>
     </row>
@@ -3055,28 +3057,28 @@
         <v>2</v>
       </c>
       <c r="C49" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="F49" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="G49" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H49" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="I49" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J49" s="3" t="s">
         <v>209</v>
-      </c>
-      <c r="D49" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="E49" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="F49" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="G49" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H49" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="I49" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="J49" s="3" t="s">
-        <v>213</v>
       </c>
       <c r="K49" s="3"/>
     </row>
@@ -3088,26 +3090,26 @@
         <v>1</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H50" s="3" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="I50" s="3"/>
       <c r="J50" s="3" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="K50" s="3"/>
     </row>
@@ -3119,26 +3121,26 @@
         <v>1</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H51" s="3" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="I51" s="3"/>
       <c r="J51" s="3" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="K51" s="3"/>
     </row>
@@ -3150,26 +3152,26 @@
         <v>2</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H52" s="3" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="I52" s="3"/>
       <c r="J52" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="K52" s="3"/>
     </row>
@@ -3181,26 +3183,26 @@
         <v>4</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H53" s="3" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="I53" s="3"/>
       <c r="J53" s="3" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="K53" s="3"/>
     </row>
@@ -3212,34 +3214,34 @@
         <v>2</v>
       </c>
       <c r="C54" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="F54" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="G54" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H54" s="3" t="s">
         <v>230</v>
-      </c>
-      <c r="D54" s="3" t="s">
-        <v>231</v>
-      </c>
-      <c r="E54" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="F54" s="3" t="s">
-        <v>233</v>
-      </c>
-      <c r="G54" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H54" s="3" t="s">
-        <v>234</v>
       </c>
       <c r="I54" s="3">
         <v>171150</v>
       </c>
       <c r="J54" s="3" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="K54" s="3"/>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.3">
@@ -3250,34 +3252,34 @@
         <v>2</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H57" s="3" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="I57" s="3" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="J57" s="3" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="K57" s="3"/>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.3">
@@ -3288,26 +3290,26 @@
         <v>4</v>
       </c>
       <c r="C60" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="F60" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="G60" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H60" s="3" t="s">
         <v>174</v>
-      </c>
-      <c r="D60" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="E60" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="F60" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="G60" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H60" s="3" t="s">
-        <v>178</v>
       </c>
       <c r="I60" s="3"/>
       <c r="J60" s="3" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="K60" s="3"/>
     </row>
@@ -3319,26 +3321,26 @@
         <v>16</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="G61" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H61" s="3" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="I61" s="3"/>
       <c r="J61" s="3" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="K61" s="3"/>
     </row>
@@ -3350,26 +3352,26 @@
         <v>40</v>
       </c>
       <c r="C62" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="F62" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="G62" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H62" s="3" t="s">
         <v>184</v>
-      </c>
-      <c r="D62" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="E62" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="F62" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="G62" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H62" s="3" t="s">
-        <v>188</v>
       </c>
       <c r="I62" s="3"/>
       <c r="J62" s="3" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="K62" s="3"/>
     </row>
@@ -3381,26 +3383,26 @@
         <v>1</v>
       </c>
       <c r="C63" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="F63" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G63" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H63" s="3" t="s">
         <v>86</v>
-      </c>
-      <c r="D63" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="E63" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="F63" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="G63" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H63" s="3" t="s">
-        <v>90</v>
       </c>
       <c r="I63" s="3"/>
       <c r="J63" s="3" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="K63" s="3"/>
     </row>

</xml_diff>